<commit_message>
Change polyfit to ployval
</commit_message>
<xml_diff>
--- a/matlab/DistanceToTy_v2.xlsx
+++ b/matlab/DistanceToTy_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithier/Documents/FIRST/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F468C35-95D5-B646-A39D-5F43DCE06614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32E5231-EC2D-004A-892E-6CEF8761A8AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19940" yWindow="0" windowWidth="13660" windowHeight="21000" xr2:uid="{03FCACD2-7F96-E54B-8934-27EB1DA6E20F}"/>
   </bookViews>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Distance from Target (in)</t>
   </si>
   <si>
     <t>ty (deg)</t>
-  </si>
-  <si>
-    <t>19..58</t>
   </si>
 </sst>
 </file>
@@ -394,7 +391,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,8 +411,8 @@
       <c r="A2">
         <v>105</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>19.579999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated excel and matlab file
</commit_message>
<xml_diff>
--- a/matlab/DistanceToTy_v2.xlsx
+++ b/matlab/DistanceToTy_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithier/Documents/FIRST/2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithier/Documents/FIRST/2020/Git/Vision2020/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F468C35-95D5-B646-A39D-5F43DCE06614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA87F90-9225-9F49-8211-E58FA987BBBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19940" yWindow="0" windowWidth="13660" windowHeight="21000" xr2:uid="{03FCACD2-7F96-E54B-8934-27EB1DA6E20F}"/>
+    <workbookView xWindow="19940" yWindow="460" windowWidth="13660" windowHeight="19540" xr2:uid="{03FCACD2-7F96-E54B-8934-27EB1DA6E20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408D842A-912E-E240-800B-BAEB3D44704C}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,6 +730,14 @@
         <v>1.89</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>350</v>
+      </c>
+      <c r="B42">
+        <v>0.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
did some error calculations on estimating distance from angle
</commit_message>
<xml_diff>
--- a/matlab/DistanceToTy_v2.xlsx
+++ b/matlab/DistanceToTy_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithier/Documents/FIRST/2020/Git/Vision2020/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213ED579-BAD8-E14A-8C0B-6D81E0A94E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC67F0-E6E5-5E43-9BF9-28486BFA17FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19940" yWindow="460" windowWidth="13660" windowHeight="19540" xr2:uid="{03FCACD2-7F96-E54B-8934-27EB1DA6E20F}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,50 +689,50 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B37">
-        <v>3.11</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B38">
-        <v>2.83</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B39">
-        <v>2.57</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B40">
-        <v>2.21</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B41">
-        <v>1.89</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B42">
-        <v>0.33</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,10 +745,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>276</v>
+        <v>350</v>
       </c>
       <c r="B44">
-        <v>3.6</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>